<commit_message>
update for january docker1
</commit_message>
<xml_diff>
--- a/lai/valuationquan/szseinnovation100index/szseinnovation100indexmodel1.xlsx
+++ b/lai/valuationquan/szseinnovation100index/szseinnovation100indexmodel1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="270">
   <si>
     <t>PE</t>
   </si>
@@ -1090,62 +1090,6 @@
   </si>
   <si>
     <t xml:space="preserve">2022/12/28
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/3
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/4
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/5
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/6
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/9
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/10
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/11
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/12
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/13
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/16
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/17
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/18
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/19
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023/1/20
 </t>
   </si>
 </sst>
@@ -1160,7 +1104,7 @@
     <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="180" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2366,11 +2310,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="324213376"/>
-        <c:axId val="324215168"/>
+        <c:axId val="245629696"/>
+        <c:axId val="245631232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="324213376"/>
+        <c:axId val="245629696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2413,7 +2357,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324215168"/>
+        <c:crossAx val="245631232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2421,7 +2365,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324215168"/>
+        <c:axId val="245631232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2472,7 +2416,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324213376"/>
+        <c:crossAx val="245629696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16662,7 +16606,7 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
@@ -16683,7 +16627,7 @@
     <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1">
+    <row r="1" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>180</v>
       </c>
@@ -16713,7 +16657,7 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:22" ht="14.1" customHeight="1">
+    <row r="2" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="4">
@@ -16729,7 +16673,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:22" ht="14.1" customHeight="1">
+    <row r="3" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>43889</v>
       </c>
@@ -16798,7 +16742,7 @@
         <v>-22000</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="14.1" customHeight="1">
+    <row r="4" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>43921</v>
       </c>
@@ -16873,7 +16817,7 @@
         <v>-24000</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="14.1" customHeight="1">
+    <row r="5" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>43951</v>
       </c>
@@ -16943,7 +16887,7 @@
         <v>53008.069006718506</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="14.1" customHeight="1">
+    <row r="6" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>43980</v>
       </c>
@@ -16985,7 +16929,7 @@
         <v>9.9835199022272558E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14.1" customHeight="1">
+    <row r="7" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>44012</v>
       </c>
@@ -17023,7 +16967,7 @@
       </c>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:22" ht="14.1" customHeight="1">
+    <row r="8" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>44043</v>
       </c>
@@ -17061,7 +17005,7 @@
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:22" ht="14.1" customHeight="1">
+    <row r="9" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>44074</v>
       </c>
@@ -17099,7 +17043,7 @@
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:22" ht="14.1" customHeight="1">
+    <row r="10" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>44104</v>
       </c>
@@ -17137,7 +17081,7 @@
       </c>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:22" ht="14.1" customHeight="1">
+    <row r="11" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>44134</v>
       </c>
@@ -17175,7 +17119,7 @@
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:22" ht="14.1" customHeight="1">
+    <row r="12" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>44165</v>
       </c>
@@ -17213,7 +17157,7 @@
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:22" ht="14.1" customHeight="1">
+    <row r="13" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>44196</v>
       </c>
@@ -17251,7 +17195,7 @@
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:22" ht="14.1" customHeight="1">
+    <row r="14" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>44225</v>
       </c>
@@ -17289,7 +17233,7 @@
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:22" ht="14.1" customHeight="1">
+    <row r="15" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>44253</v>
       </c>
@@ -17327,7 +17271,7 @@
       </c>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:22" ht="14.1" customHeight="1">
+    <row r="16" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
         <v>44286</v>
       </c>
@@ -17365,7 +17309,7 @@
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="14.1" customHeight="1">
+    <row r="17" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>44316</v>
       </c>
@@ -17403,7 +17347,7 @@
       </c>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="14.1" customHeight="1">
+    <row r="18" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
         <v>44347</v>
       </c>
@@ -17441,7 +17385,7 @@
       </c>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:12" ht="14.1" customHeight="1">
+    <row r="19" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
         <v>44377</v>
       </c>
@@ -17479,7 +17423,7 @@
       </c>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="14.1" customHeight="1">
+    <row r="20" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
         <v>44407</v>
       </c>
@@ -17517,7 +17461,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:12" ht="14.1" customHeight="1">
+    <row r="21" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
         <v>44439</v>
       </c>
@@ -17556,7 +17500,7 @@
       <c r="J21" s="6"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="14.1" customHeight="1">
+    <row r="22" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
         <v>44469</v>
       </c>
@@ -17594,7 +17538,7 @@
       </c>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:12" ht="14.1" customHeight="1">
+    <row r="23" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
         <v>44498</v>
       </c>
@@ -17632,7 +17576,7 @@
       </c>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="14.1" customHeight="1">
+    <row r="24" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
         <v>44530</v>
       </c>
@@ -17670,7 +17614,7 @@
       </c>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="14.1" customHeight="1">
+    <row r="25" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
         <v>44561</v>
       </c>
@@ -17708,7 +17652,7 @@
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:12" ht="14.1" customHeight="1">
+    <row r="26" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
         <v>44589</v>
       </c>
@@ -17746,7 +17690,7 @@
       </c>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:12" ht="14.1" customHeight="1">
+    <row r="27" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
         <v>44620</v>
       </c>
@@ -17784,7 +17728,7 @@
       </c>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="14.1" customHeight="1">
+    <row r="28" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
         <v>44651</v>
       </c>
@@ -17822,7 +17766,7 @@
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:12" ht="14.1" customHeight="1">
+    <row r="29" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
         <v>44680</v>
       </c>
@@ -17860,7 +17804,7 @@
       </c>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:12" ht="14.1" customHeight="1">
+    <row r="30" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
         <v>44712</v>
       </c>
@@ -17898,7 +17842,7 @@
       </c>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="14.1" customHeight="1">
+    <row r="31" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
         <v>44742</v>
       </c>
@@ -17936,7 +17880,7 @@
       </c>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:12" ht="14.1" customHeight="1">
+    <row r="32" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
         <v>44771</v>
       </c>
@@ -17974,7 +17918,7 @@
       </c>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:12" ht="14.1" customHeight="1">
+    <row r="33" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
         <v>44804</v>
       </c>
@@ -18013,7 +17957,7 @@
       <c r="J33" s="6"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" ht="12.75">
+    <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
         <v>44834</v>
       </c>
@@ -18050,7 +17994,7 @@
         <v>-11770.911062729705</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="12.75">
+    <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
         <v>44865</v>
       </c>
@@ -18087,7 +18031,7 @@
         <v>-12524.925264431353</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="12.75">
+    <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="14">
         <v>44895</v>
       </c>
@@ -18124,7 +18068,7 @@
         <v>-9593.1455874388703</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="12.75">
+    <row r="37" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="14">
         <v>44925</v>
       </c>
@@ -18174,13 +18118,13 @@
   <sheetPr codeName="Sheet4">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D443"/>
+  <dimension ref="A1:D427"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="18"/>
     <col min="2" max="2" width="8.5" style="18" customWidth="1"/>
@@ -18188,7 +18132,7 @@
     <col min="4" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1">
+    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="30" t="s">
         <v>194</v>
       </c>
@@ -18196,7 +18140,7 @@
         <v>399088</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1">
+    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="30"/>
       <c r="C2" s="28" t="s">
         <v>0</v>
@@ -18205,7 +18149,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1">
+    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -18220,7 +18164,7 @@
         <v>45.12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1">
+    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <f t="shared" ref="A4:A36" si="0">A3+1</f>
         <v>2</v>
@@ -18236,7 +18180,7 @@
         <v>44.965000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1">
+    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -18252,7 +18196,7 @@
         <v>44.99666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -18268,7 +18212,7 @@
         <v>44.792500000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" customHeight="1">
+    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -18284,7 +18228,7 @@
         <v>44.440000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75" customHeight="1">
+    <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -18300,7 +18244,7 @@
         <v>44.256666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1">
+    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -18316,7 +18260,7 @@
         <v>44.252857142857145</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.75" customHeight="1">
+    <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -18332,7 +18276,7 @@
         <v>44.220000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.75" customHeight="1">
+    <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -18348,7 +18292,7 @@
         <v>44.181111111111115</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.75" customHeight="1">
+    <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18364,7 +18308,7 @@
         <v>44.341000000000008</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1">
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -18380,7 +18324,7 @@
         <v>44.458181818181828</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -18396,7 +18340,7 @@
         <v>44.577500000000008</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -18412,7 +18356,7 @@
         <v>44.703076923076928</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -18428,7 +18372,7 @@
         <v>44.860000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12.75" customHeight="1">
+    <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -18444,7 +18388,7 @@
         <v>44.968000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.75" customHeight="1">
+    <row r="18" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -18460,7 +18404,7 @@
         <v>45.078750000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12.75" customHeight="1">
+    <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -18476,7 +18420,7 @@
         <v>45.214117647058828</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1">
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -18492,7 +18436,7 @@
         <v>45.345555555555563</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1">
+    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -18508,7 +18452,7 @@
         <v>45.46631578947369</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.75" customHeight="1">
+    <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -18524,7 +18468,7 @@
         <v>45.062500000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.75" customHeight="1">
+    <row r="23" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -18540,7 +18484,7 @@
         <v>44.643333333333338</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1">
+    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -18556,7 +18500,7 @@
         <v>44.269090909090913</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12.75" customHeight="1">
+    <row r="25" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -18572,7 +18516,7 @@
         <v>43.928695652173921</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12.75" customHeight="1">
+    <row r="26" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -18588,7 +18532,7 @@
         <v>43.627500000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1">
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -18604,7 +18548,7 @@
         <v>43.332400000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12.75" customHeight="1">
+    <row r="28" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -18620,7 +18564,7 @@
         <v>43.088461538461544</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="12.75" customHeight="1">
+    <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -18636,7 +18580,7 @@
         <v>42.901851851851859</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12.75" customHeight="1">
+    <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -18652,7 +18596,7 @@
         <v>42.726071428571437</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.75" customHeight="1">
+    <row r="31" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -18668,7 +18612,7 @@
         <v>42.570000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.75" customHeight="1">
+    <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -18684,7 +18628,7 @@
         <v>42.435000000000009</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="12.75" customHeight="1">
+    <row r="33" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -18700,7 +18644,7 @@
         <v>42.298387096774199</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1">
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -18716,7 +18660,7 @@
         <v>42.179062500000008</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="12.75" customHeight="1">
+    <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -18732,7 +18676,7 @@
         <v>42.093333333333341</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="12.75" customHeight="1">
+    <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -18748,7 +18692,7 @@
         <v>42.005000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="12.75" customHeight="1">
+    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <f t="shared" ref="A37:A100" si="1">A36+1</f>
         <v>35</v>
@@ -18764,7 +18708,7 @@
         <v>41.929428571428573</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="12.75" customHeight="1">
+    <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -18780,7 +18724,7 @@
         <v>41.856666666666662</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="12.75" customHeight="1">
+    <row r="39" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -18796,7 +18740,7 @@
         <v>41.802432432432425</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="12.75" customHeight="1">
+    <row r="40" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -18812,7 +18756,7 @@
         <v>41.751315789473679</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1">
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -18828,7 +18772,7 @@
         <v>41.689999999999991</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.75" customHeight="1">
+    <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -18844,7 +18788,7 @@
         <v>41.621999999999993</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="12.75" customHeight="1">
+    <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -18860,7 +18804,7 @@
         <v>41.5680487804878</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="12.75" customHeight="1">
+    <row r="44" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -18876,7 +18820,7 @@
         <v>41.512380952380944</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="12.75" customHeight="1">
+    <row r="45" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -18892,7 +18836,7 @@
         <v>41.454186046511623</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="12.75" customHeight="1">
+    <row r="46" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -18908,7 +18852,7 @@
         <v>41.399318181818174</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="12.75" customHeight="1">
+    <row r="47" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -18924,7 +18868,7 @@
         <v>41.36044444444444</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1">
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -18940,7 +18884,7 @@
         <v>41.322391304347818</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="12.75" customHeight="1">
+    <row r="49" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -18956,7 +18900,7 @@
         <v>41.285319148936161</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.75" customHeight="1">
+    <row r="50" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -18972,7 +18916,7 @@
         <v>41.222499999999989</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="12.75" customHeight="1">
+    <row r="51" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -18988,7 +18932,7 @@
         <v>41.174693877551015</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="12.75" customHeight="1">
+    <row r="52" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -19004,7 +18948,7 @@
         <v>41.139199999999988</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="12.75" customHeight="1">
+    <row r="53" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -19020,7 +18964,7 @@
         <v>41.106862745098027</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="12.75" customHeight="1">
+    <row r="54" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -19036,7 +18980,7 @@
         <v>41.078653846153834</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1">
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -19052,7 +18996,7 @@
         <v>41.062452830188661</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="12.75" customHeight="1">
+    <row r="56" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -19068,7 +19012,7 @@
         <v>41.045555555555538</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="12.75" customHeight="1">
+    <row r="57" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -19084,7 +19028,7 @@
         <v>41.038181818181798</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="12.75" customHeight="1">
+    <row r="58" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -19100,7 +19044,7 @@
         <v>41.038928571428549</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="12.75" customHeight="1">
+    <row r="59" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -19116,7 +19060,7 @@
         <v>41.034736842105247</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="12.75" customHeight="1">
+    <row r="60" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -19132,7 +19076,7 @@
         <v>41.041896551724122</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="12.75" customHeight="1">
+    <row r="61" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -19148,7 +19092,7 @@
         <v>41.046101694915237</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1">
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -19164,7 +19108,7 @@
         <v>41.029166666666654</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="12.75" customHeight="1">
+    <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -19180,7 +19124,7 @@
         <v>41.015737704918017</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="12.75" customHeight="1">
+    <row r="64" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -19196,7 +19140,7 @@
         <v>40.997580645161271</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12.75" customHeight="1">
+    <row r="65" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -19212,7 +19156,7 @@
         <v>40.997301587301571</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="12.75" customHeight="1">
+    <row r="66" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -19228,7 +19172,7 @@
         <v>40.998281249999984</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="12.75" customHeight="1">
+    <row r="67" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -19244,7 +19188,7 @@
         <v>40.994153846153829</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="12.75" customHeight="1">
+    <row r="68" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -19260,7 +19204,7 @@
         <v>41.006060606060593</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1">
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -19276,7 +19220,7 @@
         <v>41.01641791044775</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="12.75" customHeight="1">
+    <row r="70" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -19292,7 +19236,7 @@
         <v>41.020294117647047</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="12.75" customHeight="1">
+    <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -19308,7 +19252,7 @@
         <v>41.027826086956509</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="12.75" customHeight="1">
+    <row r="72" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -19324,7 +19268,7 @@
         <v>41.021428571428558</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="12.75" customHeight="1">
+    <row r="73" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -19340,7 +19284,7 @@
         <v>41.019295774647873</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="12.75" customHeight="1">
+    <row r="74" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -19356,7 +19300,7 @@
         <v>41.017499999999984</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="12.75" customHeight="1">
+    <row r="75" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -19372,7 +19316,7 @@
         <v>41.027123287671216</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1">
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -19388,7 +19332,7 @@
         <v>41.036081081081065</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="12.75" customHeight="1">
+    <row r="77" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -19404,7 +19348,7 @@
         <v>41.035466666666643</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="12.75" customHeight="1">
+    <row r="78" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -19420,7 +19364,7 @@
         <v>41.020526335866805</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="12.75" customHeight="1">
+    <row r="79" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -19436,7 +19380,7 @@
         <v>40.984025981952598</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="12.75" customHeight="1">
+    <row r="80" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -19452,7 +19396,7 @@
         <v>40.953717942849167</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="12.75" customHeight="1">
+    <row r="81" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -19468,7 +19412,7 @@
         <v>40.943164537647085</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="12.75" customHeight="1">
+    <row r="82" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="18">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -19484,7 +19428,7 @@
         <v>40.930499984741189</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="12.75" customHeight="1">
+    <row r="83" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -19500,7 +19444,7 @@
         <v>40.927160476872935</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="12.75" customHeight="1">
+    <row r="84" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -19516,7 +19460,7 @@
         <v>40.921951202764724</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="12.75" customHeight="1">
+    <row r="85" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="18">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -19532,7 +19476,7 @@
         <v>40.929036107810127</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="12.75" customHeight="1">
+    <row r="86" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="18">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -19548,7 +19492,7 @@
         <v>40.931428547813759</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="12.75" customHeight="1">
+    <row r="87" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="18">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -19564,7 +19508,7 @@
         <v>40.92988232062843</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="12.75" customHeight="1">
+    <row r="88" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="18">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -19580,7 +19524,7 @@
         <v>40.928372052214847</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="12.75" customHeight="1">
+    <row r="89" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="18">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -19596,7 +19540,7 @@
         <v>40.927701096808754</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="12.75" customHeight="1">
+    <row r="90" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -19612,7 +19556,7 @@
         <v>40.924090864008107</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="12.75" customHeight="1">
+    <row r="91" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -19628,7 +19572,7 @@
         <v>40.917528047025854</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="12.75" customHeight="1">
+    <row r="92" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="18">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -19644,7 +19588,7 @@
         <v>40.904444420708536</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="12.75" customHeight="1">
+    <row r="93" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="18">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -19660,7 +19604,7 @@
         <v>40.886703283288959</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="12.75" customHeight="1">
+    <row r="94" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="18">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -19676,7 +19620,7 @@
         <v>40.859891271176529</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="12.75" customHeight="1">
+    <row r="95" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="18">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -19692,7 +19636,7 @@
         <v>40.836344033518131</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="12.75" customHeight="1">
+    <row r="96" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="18">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -19708,7 +19652,7 @@
         <v>40.815851010261682</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="12.75" customHeight="1">
+    <row r="97" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="18">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -19724,7 +19668,7 @@
         <v>40.787684151097331</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="12.75" customHeight="1">
+    <row r="98" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="18">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -19740,7 +19684,7 @@
         <v>40.770416618982935</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="12.75" customHeight="1">
+    <row r="99" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="18">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -19756,7 +19700,7 @@
         <v>40.756804084384548</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="12.75" customHeight="1">
+    <row r="100" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="18">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -19772,7 +19716,7 @@
         <v>40.744489749207773</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="12.75" customHeight="1">
+    <row r="101" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="18">
         <f t="shared" ref="A101:A355" si="2">A100+1</f>
         <v>99</v>
@@ -19788,7 +19732,7 @@
         <v>40.723232270828383</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="12.75" customHeight="1">
+    <row r="102" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="18">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -19804,7 +19748,7 @@
         <v>40.702299958801255</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="12.75" customHeight="1">
+    <row r="103" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="18">
         <f t="shared" si="2"/>
         <v>101</v>
@@ -19820,7 +19764,7 @@
         <v>40.680296984379815</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="12.75" customHeight="1">
+    <row r="104" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="18">
         <f t="shared" si="2"/>
         <v>102</v>
@@ -19836,7 +19780,7 @@
         <v>40.654705834482208</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="12.75" customHeight="1">
+    <row r="105" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="18">
         <f t="shared" si="2"/>
         <v>103</v>
@@ -19852,7 +19796,7 @@
         <v>40.599999957038342</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="12.75" customHeight="1">
+    <row r="106" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="18">
         <f t="shared" si="2"/>
         <v>104</v>
@@ -19868,7 +19812,7 @@
         <v>40.542692259274979</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="12.75" customHeight="1">
+    <row r="107" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="18">
         <f t="shared" si="2"/>
         <v>105</v>
@@ -19884,7 +19828,7 @@
         <v>40.482476154145722</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="12.75" customHeight="1">
+    <row r="108" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="18">
         <f t="shared" si="2"/>
         <v>106</v>
@@ -19900,7 +19844,7 @@
         <v>40.435849029253099</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="12.75" customHeight="1">
+    <row r="109" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="18">
         <f t="shared" si="2"/>
         <v>107</v>
@@ -19916,7 +19860,7 @@
         <v>40.391775685247957</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="12.75" customHeight="1">
+    <row r="110" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="18">
         <f t="shared" si="2"/>
         <v>108</v>
@@ -19932,7 +19876,7 @@
         <v>40.346574042991335</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="12.75" customHeight="1">
+    <row r="111" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="18">
         <f t="shared" si="2"/>
         <v>109</v>
@@ -19948,7 +19892,7 @@
         <v>40.302110060945544</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="12.75" customHeight="1">
+    <row r="112" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="18">
         <f t="shared" si="2"/>
         <v>110</v>
@@ -19964,7 +19908,7 @@
         <v>40.260272703690944</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="12.75" customHeight="1">
+    <row r="113" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="18">
         <f t="shared" si="2"/>
         <v>111</v>
@@ -19980,7 +19924,7 @@
         <v>40.215585555342926</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="12.75" customHeight="1">
+    <row r="114" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="18">
         <f t="shared" si="2"/>
         <v>112</v>
@@ -19996,7 +19940,7 @@
         <v>40.173214266640784</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="12.75" customHeight="1">
+    <row r="115" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="18">
         <f t="shared" si="2"/>
         <v>113</v>
@@ -20012,7 +19956,7 @@
         <v>40.128584061344093</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="12.75" customHeight="1">
+    <row r="116" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="18">
         <f t="shared" si="2"/>
         <v>114</v>
@@ -20028,7 +19972,7 @@
         <v>40.078245599311678</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="12.75" customHeight="1">
+    <row r="117" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="18">
         <f t="shared" si="2"/>
         <v>115</v>
@@ -20044,7 +19988,7 @@
         <v>40.032521721881352</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="12.75" customHeight="1">
+    <row r="118" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="18">
         <f t="shared" si="2"/>
         <v>116</v>
@@ -20060,7 +20004,7 @@
         <v>39.985344822324535</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="12.75" customHeight="1">
+    <row r="119" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="18">
         <f t="shared" si="2"/>
         <v>117</v>
@@ -20076,7 +20020,7 @@
         <v>39.940427341298147</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="12.75" customHeight="1">
+    <row r="120" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="18">
         <f t="shared" si="2"/>
         <v>118</v>
@@ -20092,7 +20036,7 @@
         <v>39.89703388666701</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="12.75" customHeight="1">
+    <row r="121" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="18">
         <f t="shared" si="2"/>
         <v>119</v>
@@ -20108,7 +20052,7 @@
         <v>39.856638645204157</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="12.75" customHeight="1">
+    <row r="122" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="18">
         <f t="shared" si="2"/>
         <v>120</v>
@@ -20124,7 +20068,7 @@
         <v>39.814833324432357</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="12.75" customHeight="1">
+    <row r="123" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="18">
         <f t="shared" si="2"/>
         <v>121</v>
@@ -20140,7 +20084,7 @@
         <v>39.769752062332515</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="12.75" customHeight="1">
+    <row r="124" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="18">
         <f t="shared" si="2"/>
         <v>122</v>
@@ -20156,7 +20100,7 @@
         <v>39.730819672131133</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="12.75" customHeight="1">
+    <row r="125" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="18">
         <f t="shared" si="2"/>
         <v>123</v>
@@ -20172,7 +20116,7 @@
         <v>39.694634136422749</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="12.75" customHeight="1">
+    <row r="126" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="18">
         <f t="shared" si="2"/>
         <v>124</v>
@@ -20188,7 +20132,7 @@
         <v>39.656854815322561</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="12.75" customHeight="1">
+    <row r="127" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="18">
         <f t="shared" si="2"/>
         <v>125</v>
@@ -20204,7 +20148,7 @@
         <v>39.615839967039982</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="12.75" customHeight="1">
+    <row r="128" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="18">
         <f t="shared" si="2"/>
         <v>126</v>
@@ -20220,7 +20164,7 @@
         <v>39.58039680484125</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="12.75" customHeight="1">
+    <row r="129" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="18">
         <f t="shared" si="2"/>
         <v>127</v>
@@ -20236,7 +20180,7 @@
         <v>39.545433045669277</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="12.75" customHeight="1">
+    <row r="130" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="18">
         <f t="shared" si="2"/>
         <v>128</v>
@@ -20252,7 +20196,7 @@
         <v>39.514765591640611</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="12.75" customHeight="1">
+    <row r="131" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="18">
         <f t="shared" si="2"/>
         <v>129</v>
@@ -20268,7 +20212,7 @@
         <v>39.483953462403086</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="12.75" customHeight="1">
+    <row r="132" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="18">
         <f t="shared" si="2"/>
         <v>130</v>
@@ -20284,7 +20228,7 @@
         <v>39.455384593153838</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="12.75" customHeight="1">
+    <row r="133" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="18">
         <f t="shared" si="2"/>
         <v>131</v>
@@ -20300,7 +20244,7 @@
         <v>39.425419815954186</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="12.75" customHeight="1">
+    <row r="134" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="18">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -20316,7 +20260,7 @@
         <v>39.396590869848474</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="12.75" customHeight="1">
+    <row r="135" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="18">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -20332,7 +20276,7 @@
         <v>39.371127767969917</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="12.75" customHeight="1">
+    <row r="136" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="18">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -20348,7 +20292,7 @@
         <v>39.348358155447755</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="12.75" customHeight="1">
+    <row r="137" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="18">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -20364,7 +20308,7 @@
         <v>39.325777719037028</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="12.75" customHeight="1">
+    <row r="138" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="18">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -20380,7 +20324,7 @@
         <v>39.30124995404411</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="12.75" customHeight="1">
+    <row r="139" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="18">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -20396,7 +20340,7 @@
         <v>39.275182432773718</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="12.75" customHeight="1">
+    <row r="140" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="18">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -20412,7 +20356,7 @@
         <v>39.253623134275358</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="12.75" customHeight="1">
+    <row r="141" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="18">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -20428,7 +20372,7 @@
         <v>39.222517934100708</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="12.75" customHeight="1">
+    <row r="142" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="18">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -20444,7 +20388,7 @@
         <v>39.191714233499987</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="12.75" customHeight="1">
+    <row r="143" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="18">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -20460,7 +20404,7 @@
         <v>39.159361657872324</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="12.75" customHeight="1">
+    <row r="144" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="18">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -20476,7 +20420,7 @@
         <v>39.130704182464775</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="12.75" customHeight="1">
+    <row r="145" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="18">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -20492,7 +20436,7 @@
         <v>39.101118849230758</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="12.75" customHeight="1">
+    <row r="146" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="18">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -20508,7 +20452,7 @@
         <v>39.072916641388879</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="12.75" customHeight="1">
+    <row r="147" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="18">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -20524,7 +20468,7 @@
         <v>39.046344810896542</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="12.75" customHeight="1">
+    <row r="148" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="18">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -20540,7 +20484,7 @@
         <v>39.018561638767117</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="12.75" customHeight="1">
+    <row r="149" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="18">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -20556,7 +20500,7 @@
         <v>38.994013599387742</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="12.75" customHeight="1">
+    <row r="150" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="18">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -20572,7 +20516,7 @@
         <v>38.968783766418909</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="12.75" customHeight="1">
+    <row r="151" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="18">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -20588,7 +20532,7 @@
         <v>38.941812068389247</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="12.75" customHeight="1">
+    <row r="152" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="18">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -20604,7 +20548,7 @@
         <v>38.915199992999987</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="12.75" customHeight="1">
+    <row r="153" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="18">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -20620,7 +20564,7 @@
         <v>38.890794691986741</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="12.75" customHeight="1">
+    <row r="154" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="18">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -20636,7 +20580,7 @@
         <v>38.864144727894725</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="12.75" customHeight="1">
+    <row r="155" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="18">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -20652,7 +20596,7 @@
         <v>38.840653588888877</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="12.75" customHeight="1">
+    <row r="156" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="18">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -20668,7 +20612,7 @@
         <v>38.822142862207784</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="12.75" customHeight="1">
+    <row r="157" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="18">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -20684,7 +20628,7 @@
         <v>38.801870974774182</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="12.75" customHeight="1">
+    <row r="158" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="18">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -20700,7 +20644,7 @@
         <v>38.781025643141014</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="12.75" customHeight="1">
+    <row r="159" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="18">
         <f t="shared" si="2"/>
         <v>157</v>
@@ -20716,7 +20660,7 @@
         <v>38.75942674980891</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="12.75" customHeight="1">
+    <row r="160" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="18">
         <f t="shared" si="2"/>
         <v>158</v>
@@ -20732,7 +20676,7 @@
         <v>38.73683543259493</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="12.75" customHeight="1">
+    <row r="161" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="18">
         <f t="shared" si="2"/>
         <v>159</v>
@@ -20748,7 +20692,7 @@
         <v>38.715911938364776</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="12.75" customHeight="1">
+    <row r="162" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="18">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -20764,7 +20708,7 @@
         <v>38.695499988749994</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="12.75" customHeight="1">
+    <row r="163" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="18">
         <f t="shared" si="2"/>
         <v>161</v>
@@ -20780,7 +20724,7 @@
         <v>38.674285695527942</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="12.75" customHeight="1">
+    <row r="164" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="18">
         <f t="shared" si="2"/>
         <v>162</v>
@@ -20796,7 +20740,7 @@
         <v>38.652962951851848</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="12.75" customHeight="1">
+    <row r="165" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="18">
         <f t="shared" si="2"/>
         <v>163</v>
@@ -20812,7 +20756,7 @@
         <v>38.632515324478518</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="12.75" customHeight="1">
+    <row r="166" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="18">
         <f t="shared" si="2"/>
         <v>164</v>
@@ -20828,7 +20772,7 @@
         <v>38.609999978780486</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="12.75" customHeight="1">
+    <row r="167" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="18">
         <f t="shared" si="2"/>
         <v>165</v>
@@ -20844,7 +20788,7 @@
         <v>38.586363609696967</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="12.75" customHeight="1">
+    <row r="168" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="18">
         <f t="shared" si="2"/>
         <v>166</v>
@@ -20860,7 +20804,7 @@
         <v>38.566746972469872</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="12.75" customHeight="1">
+    <row r="169" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="18">
         <f t="shared" si="2"/>
         <v>167</v>
@@ -20876,7 +20820,7 @@
         <v>38.550598780598797</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="12.75" customHeight="1">
+    <row r="170" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="18">
         <f t="shared" si="2"/>
         <v>168</v>
@@ -20892,7 +20836,7 @@
         <v>38.53458331529761</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="12.75" customHeight="1">
+    <row r="171" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="18">
         <f t="shared" si="2"/>
         <v>169</v>
@@ -20908,7 +20852,7 @@
         <v>38.518757382130168</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="12.75" customHeight="1">
+    <row r="172" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="18">
         <f t="shared" si="2"/>
         <v>170</v>
@@ -20924,7 +20868,7 @@
         <v>38.501588212058813</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="12.75" customHeight="1">
+    <row r="173" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="18">
         <f t="shared" si="2"/>
         <v>171</v>
@@ -20940,7 +20884,7 @@
         <v>38.482806999824554</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="12.75" customHeight="1">
+    <row r="174" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="18">
         <f t="shared" si="2"/>
         <v>172</v>
@@ -20956,7 +20900,7 @@
         <v>38.465581380406974</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="12.75" customHeight="1">
+    <row r="175" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="18">
         <f t="shared" si="2"/>
         <v>173</v>
@@ -20972,7 +20916,7 @@
         <v>38.445202289364161</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="12.75" customHeight="1">
+    <row r="176" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="18">
         <f t="shared" si="2"/>
         <v>174</v>
@@ -20988,7 +20932,7 @@
         <v>38.42022985362069</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="12.75" customHeight="1">
+    <row r="177" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="18">
         <f t="shared" si="2"/>
         <v>175</v>
@@ -21004,7 +20948,7 @@
         <v>38.397485675200002</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="12.75" customHeight="1">
+    <row r="178" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="18">
         <f t="shared" si="2"/>
         <v>176</v>
@@ -21020,7 +20964,7 @@
         <v>38.376420407897733</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="12.75" customHeight="1">
+    <row r="179" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="18">
         <f t="shared" si="2"/>
         <v>177</v>
@@ -21036,7 +20980,7 @@
         <v>38.356271147796612</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="12.75" customHeight="1">
+    <row r="180" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="18">
         <f t="shared" si="2"/>
         <v>178</v>
@@ -21052,7 +20996,7 @@
         <v>38.333426933033707</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="12.75" customHeight="1">
+    <row r="181" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="18">
         <f t="shared" si="2"/>
         <v>179</v>
@@ -21068,7 +21012,7 @@
         <v>38.311229020614526</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="12.75" customHeight="1">
+    <row r="182" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="18">
         <f t="shared" si="2"/>
         <v>180</v>
@@ -21084,7 +21028,7 @@
         <v>38.290888867888889</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="12.75" customHeight="1">
+    <row r="183" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="18">
         <f t="shared" si="2"/>
         <v>181</v>
@@ -21100,7 +21044,7 @@
         <v>38.268618754364638</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="12.75" customHeight="1">
+    <row r="184" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="18">
         <f t="shared" si="2"/>
         <v>182</v>
@@ -21116,7 +21060,7 @@
         <v>38.248351618351641</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="12.75" customHeight="1">
+    <row r="185" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="18">
         <f t="shared" si="2"/>
         <v>183</v>
@@ -21132,7 +21076,7 @@
         <v>38.228579205136612</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="12.75" customHeight="1">
+    <row r="186" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="18">
         <f t="shared" si="2"/>
         <v>184</v>
@@ -21148,7 +21092,7 @@
         <v>38.206847793913042</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="12.75" customHeight="1">
+    <row r="187" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="18">
         <f t="shared" si="2"/>
         <v>185</v>
@@ -21164,7 +21108,7 @@
         <v>38.181189152216213</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="12.75" customHeight="1">
+    <row r="188" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="18">
         <f t="shared" si="2"/>
         <v>186</v>
@@ -21180,7 +21124,7 @@
         <v>38.15387092274193</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="12.75" customHeight="1">
+    <row r="189" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="18">
         <f t="shared" si="2"/>
         <v>187</v>
@@ -21196,7 +21140,7 @@
         <v>38.12657749128342</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="12.75" customHeight="1">
+    <row r="190" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="18">
         <f t="shared" si="2"/>
         <v>188</v>
@@ -21212,7 +21156,7 @@
         <v>38.100053139680853</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="12.75" customHeight="1">
+    <row r="191" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="18">
         <f t="shared" si="2"/>
         <v>189</v>
@@ -21228,7 +21172,7 @@
         <v>38.071216879682538</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="12.75" customHeight="1">
+    <row r="192" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="18">
         <f t="shared" si="2"/>
         <v>190</v>
@@ -21244,7 +21188,7 @@
         <v>38.0456315228421</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="12.75" customHeight="1">
+    <row r="193" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="18">
         <f t="shared" si="2"/>
         <v>191</v>
@@ -21260,7 +21204,7 @@
         <v>38.017120363036646</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="12.75" customHeight="1">
+    <row r="194" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="18">
         <f t="shared" si="2"/>
         <v>192</v>
@@ -21276,7 +21220,7 @@
         <v>37.989791613541662</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="12.75" customHeight="1">
+    <row r="195" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="18">
         <f t="shared" si="2"/>
         <v>193</v>
@@ -21292,7 +21236,7 @@
         <v>37.965699429792743</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="12.75" customHeight="1">
+    <row r="196" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="18">
         <f t="shared" si="2"/>
         <v>194</v>
@@ -21308,7 +21252,7 @@
         <v>37.941855619072165</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="12.75" customHeight="1">
+    <row r="197" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="18">
         <f t="shared" si="2"/>
         <v>195</v>
@@ -21324,7 +21268,7 @@
         <v>37.915128152000001</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="12.75" customHeight="1">
+    <row r="198" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="18">
         <f t="shared" si="2"/>
         <v>196</v>
@@ -21340,7 +21284,7 @@
         <v>37.889132598622453</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="12.75" customHeight="1">
+    <row r="199" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="18">
         <f t="shared" si="2"/>
         <v>197</v>
@@ -21356,7 +21300,7 @@
         <v>37.861268989137059</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="12.75" customHeight="1">
+    <row r="200" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="18">
         <f t="shared" si="2"/>
         <v>198</v>
@@ -21372,7 +21316,7 @@
         <v>37.834646419242425</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="12.75" customHeight="1">
+    <row r="201" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="18">
         <f t="shared" si="2"/>
         <v>199</v>
@@ -21388,7 +21332,7 @@
         <v>37.804422063819104</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="12.75" customHeight="1">
+    <row r="202" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="18">
         <f t="shared" si="2"/>
         <v>200</v>
@@ -21404,7 +21348,7 @@
         <v>37.775999948150009</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="12.75" customHeight="1">
+    <row r="203" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="18">
         <f t="shared" si="2"/>
         <v>201</v>
@@ -21420,7 +21364,7 @@
         <v>37.743084524776123</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="12.75" customHeight="1">
+    <row r="204" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="18">
         <f t="shared" si="2"/>
         <v>202</v>
@@ -21436,7 +21380,7 @@
         <v>37.710494996683174</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="12.75" customHeight="1">
+    <row r="205" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="18">
         <f t="shared" si="2"/>
         <v>203</v>
@@ -21452,7 +21396,7 @@
         <v>37.678472849310346</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="12.75" customHeight="1">
+    <row r="206" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="18">
         <f t="shared" si="2"/>
         <v>204</v>
@@ -21468,7 +21412,7 @@
         <v>37.643872496323532</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="12.75" customHeight="1">
+    <row r="207" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="18">
         <f t="shared" si="2"/>
         <v>205</v>
@@ -21484,7 +21428,7 @@
         <v>37.61151214380488</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="12.75" customHeight="1">
+    <row r="208" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="18">
         <f t="shared" si="2"/>
         <v>206</v>
@@ -21500,7 +21444,7 @@
         <v>37.577281499757277</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="12.75" customHeight="1">
+    <row r="209" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="18">
         <f t="shared" si="2"/>
         <v>207</v>
@@ -21516,7 +21460,7 @@
         <v>37.540193181497585</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="12.75" customHeight="1">
+    <row r="210" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="18">
         <f t="shared" si="2"/>
         <v>208</v>
@@ -21532,7 +21476,7 @@
         <v>37.503221100721149</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="12.75" customHeight="1">
+    <row r="211" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="18">
         <f t="shared" si="2"/>
         <v>209</v>
@@ -21548,7 +21492,7 @@
         <v>37.469999944593297</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="12.75" customHeight="1">
+    <row r="212" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="18">
         <f t="shared" si="2"/>
         <v>210</v>
@@ -21564,7 +21508,7 @@
         <v>37.437380901238093</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="12.75" customHeight="1">
+    <row r="213" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="18">
         <f t="shared" si="2"/>
         <v>211</v>
@@ -21580,7 +21524,7 @@
         <v>37.405781941800946</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="12.75" customHeight="1">
+    <row r="214" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="18">
         <f t="shared" si="2"/>
         <v>212</v>
@@ -21596,7 +21540,7 @@
         <v>37.374245231273584</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="12.75" customHeight="1">
+    <row r="215" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="18">
         <f t="shared" si="2"/>
         <v>213</v>
@@ -21612,7 +21556,7 @@
         <v>37.342629053615028</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="12.75" customHeight="1">
+    <row r="216" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="18">
         <f t="shared" si="2"/>
         <v>214</v>
@@ -21628,7 +21572,7 @@
         <v>37.309205555841125</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="12.75" customHeight="1">
+    <row r="217" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="18">
         <f t="shared" si="2"/>
         <v>215</v>
@@ -21644,7 +21588,7 @@
         <v>37.27981390102326</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="12.75" customHeight="1">
+    <row r="218" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="18">
         <f t="shared" si="2"/>
         <v>216</v>
@@ -21660,7 +21604,7 @@
         <v>37.247685133657413</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="12.75" customHeight="1">
+    <row r="219" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="18">
         <f t="shared" si="2"/>
         <v>217</v>
@@ -21676,7 +21620,7 @@
         <v>37.218433126682037</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="12.75" customHeight="1">
+    <row r="220" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="18">
         <f t="shared" si="2"/>
         <v>218</v>
@@ -21692,7 +21636,7 @@
         <v>37.189770586238538</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="12.75" customHeight="1">
+    <row r="221" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="18">
         <f t="shared" si="2"/>
         <v>219</v>
@@ -21708,7 +21652,7 @@
         <v>37.161232823424669</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="12.75" customHeight="1">
+    <row r="222" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="18">
         <f t="shared" si="2"/>
         <v>220</v>
@@ -21724,7 +21668,7 @@
         <v>37.130772670045459</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="12.75" customHeight="1">
+    <row r="223" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="18">
         <f t="shared" si="2"/>
         <v>221</v>
@@ -21740,7 +21684,7 @@
         <v>37.098913970859734</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="12.75" customHeight="1">
+    <row r="224" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="18">
         <f t="shared" si="2"/>
         <v>222</v>
@@ -21756,7 +21700,7 @@
         <v>37.065180126891896</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="12.75" customHeight="1">
+    <row r="225" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="18">
         <f t="shared" si="2"/>
         <v>223</v>
@@ -21772,7 +21716,7 @@
         <v>37.026053759282519</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="12.75" customHeight="1">
+    <row r="226" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="18">
         <f t="shared" si="2"/>
         <v>224</v>
@@ -21788,7 +21732,7 @@
         <v>36.984464229464287</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="12.75" customHeight="1">
+    <row r="227" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="18">
         <f t="shared" si="2"/>
         <v>225</v>
@@ -21804,7 +21748,7 @@
         <v>36.94248883697778</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="12.75" customHeight="1">
+    <row r="228" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="18">
         <f t="shared" si="2"/>
         <v>226</v>
@@ -21820,7 +21764,7 @@
         <v>36.903849501769912</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="12.75" customHeight="1">
+    <row r="229" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="18">
         <f t="shared" si="2"/>
         <v>227</v>
@@ -21836,7 +21780,7 @@
         <v>36.866607877356834</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="12.75" customHeight="1">
+    <row r="230" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="18">
         <f t="shared" si="2"/>
         <v>228</v>
@@ -21852,7 +21796,7 @@
         <v>36.825438542543864</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="12.75" customHeight="1">
+    <row r="231" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="18">
         <f t="shared" si="2"/>
         <v>229</v>
@@ -21868,7 +21812,7 @@
         <v>36.780523967772936</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="12.75" customHeight="1">
+    <row r="232" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="18">
         <f t="shared" si="2"/>
         <v>230</v>
@@ -21884,7 +21828,7 @@
         <v>36.740956473608705</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="12.75" customHeight="1">
+    <row r="233" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="18">
         <f t="shared" si="2"/>
         <v>231</v>
@@ -21900,7 +21844,7 @@
         <v>36.704978308398275</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="12.75" customHeight="1">
+    <row r="234" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="18">
         <f t="shared" si="2"/>
         <v>232</v>
@@ -21916,7 +21860,7 @@
         <v>36.66892236806035</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="12.75" customHeight="1">
+    <row r="235" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="18">
         <f t="shared" si="2"/>
         <v>233</v>
@@ -21932,7 +21876,7 @@
         <v>36.633948454291847</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="12.75" customHeight="1">
+    <row r="236" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="18">
         <f t="shared" si="2"/>
         <v>234</v>
@@ -21948,7 +21892,7 @@
         <v>36.598119614743588</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="12.75" customHeight="1">
+    <row r="237" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="18">
         <f t="shared" si="2"/>
         <v>235</v>
@@ -21964,7 +21908,7 @@
         <v>36.563361660255318</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="12.75" customHeight="1">
+    <row r="238" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="18">
         <f t="shared" si="2"/>
         <v>236</v>
@@ -21980,7 +21924,7 @@
         <v>36.528262673093217</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="12.75" customHeight="1">
+    <row r="239" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="18">
         <f t="shared" si="2"/>
         <v>237</v>
@@ -21996,7 +21940,7 @@
         <v>36.490632875358649</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="12.75" customHeight="1">
+    <row r="240" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="18">
         <f t="shared" si="2"/>
         <v>238</v>
@@ -22012,7 +21956,7 @@
         <v>36.451512570462185</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="12.75" customHeight="1">
+    <row r="241" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="18">
         <f t="shared" si="2"/>
         <v>239</v>
@@ -22028,7 +21972,7 @@
         <v>36.412008334728036</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="12.75" customHeight="1">
+    <row r="242" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="18">
         <f t="shared" si="2"/>
         <v>240</v>
@@ -22044,7 +21988,7 @@
         <v>36.376874964750002</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="12.75" customHeight="1">
+    <row r="243" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="18">
         <f t="shared" si="2"/>
         <v>241</v>
@@ -22060,7 +22004,7 @@
         <v>36.340622369004151</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="12.75" customHeight="1">
+    <row r="244" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="18">
         <f t="shared" si="2"/>
         <v>242</v>
@@ -22076,7 +22020,7 @@
         <v>36.305495830909088</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="12.75" customHeight="1">
+    <row r="245" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="18">
         <f t="shared" si="2"/>
         <v>243</v>
@@ -22092,7 +22036,7 @@
         <v>36.269876504938274</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="12.75" customHeight="1">
+    <row r="246" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="18">
         <f t="shared" si="2"/>
         <v>244</v>
@@ -22108,7 +22052,7 @@
         <v>36.232704883032788</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="12.75" customHeight="1">
+    <row r="247" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="18">
         <f t="shared" si="2"/>
         <v>245</v>
@@ -22124,7 +22068,7 @@
         <v>36.195714251183674</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="12.75" customHeight="1">
+    <row r="248" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="18">
         <f t="shared" si="2"/>
         <v>246</v>
@@ -22140,7 +22084,7 @@
         <v>36.154715415243899</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="12.75" customHeight="1">
+    <row r="249" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="18">
         <f t="shared" si="2"/>
         <v>247</v>
@@ -22156,7 +22100,7 @@
         <v>36.116113331943318</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="12.75" customHeight="1">
+    <row r="250" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="18">
         <f t="shared" si="2"/>
         <v>248</v>
@@ -22172,7 +22116,7 @@
         <v>36.076048360080641</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="12.75" customHeight="1">
+    <row r="251" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="18">
         <f t="shared" si="2"/>
         <v>249</v>
@@ -22188,7 +22132,7 @@
         <v>36.036947764859427</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="12.75" customHeight="1">
+    <row r="252" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="18">
         <f t="shared" si="2"/>
         <v>250</v>
@@ -22204,7 +22148,7 @@
         <v>35.997639970119991</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="12.75" customHeight="1">
+    <row r="253" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="18">
         <f t="shared" si="2"/>
         <v>251</v>
@@ -22220,7 +22164,7 @@
         <v>35.959402359163342</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="12.75" customHeight="1">
+    <row r="254" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="18">
         <f t="shared" si="2"/>
         <v>252</v>
@@ -22236,7 +22180,7 @@
         <v>35.920357115039671</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="12.75" customHeight="1">
+    <row r="255" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="18">
         <f t="shared" si="2"/>
         <v>253</v>
@@ -22252,7 +22196,7 @@
         <v>35.879051352964417</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="12.75" customHeight="1">
+    <row r="256" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="18">
         <f t="shared" si="2"/>
         <v>254</v>
@@ -22268,7 +22212,7 @@
         <v>35.835787368858256</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="12.75" customHeight="1">
+    <row r="257" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="18">
         <f t="shared" si="2"/>
         <v>255</v>
@@ -22284,7 +22228,7 @@
         <v>35.792862710117632</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="12.75" customHeight="1">
+    <row r="258" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="18">
         <f t="shared" si="2"/>
         <v>256</v>
@@ -22300,7 +22244,7 @@
         <v>35.744648405624986</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="12.75" customHeight="1">
+    <row r="259" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="18">
         <f t="shared" si="2"/>
         <v>257</v>
@@ -22316,7 +22260,7 @@
         <v>35.69571981291827</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="12.75" customHeight="1">
+    <row r="260" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="18">
         <f t="shared" si="2"/>
         <v>258</v>
@@ -22332,7 +22276,7 @@
         <v>35.651472839573628</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="12.75" customHeight="1">
+    <row r="261" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="18">
         <f t="shared" si="2"/>
         <v>259</v>
@@ -22348,7 +22292,7 @@
         <v>35.606949781660212</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="12.75" customHeight="1">
+    <row r="262" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="18">
         <f t="shared" si="2"/>
         <v>260</v>
@@ -22364,7 +22308,7 @@
         <v>35.566653817730753</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="12.75" customHeight="1">
+    <row r="263" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="18">
         <f t="shared" si="2"/>
         <v>261</v>
@@ -22380,7 +22324,7 @@
         <v>35.519386943103434</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="12.75" customHeight="1">
+    <row r="264" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="18">
         <f t="shared" si="2"/>
         <v>262</v>
@@ -22396,7 +22340,7 @@
         <v>35.470534318549603</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="12.75" customHeight="1">
+    <row r="265" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="18">
         <f t="shared" si="2"/>
         <v>263</v>
@@ -22412,7 +22356,7 @@
         <v>35.421064602813672</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="12.75" customHeight="1">
+    <row r="266" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="18">
         <f t="shared" si="2"/>
         <v>264</v>
@@ -22428,7 +22372,7 @@
         <v>35.373181784962107</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="12.75" customHeight="1">
+    <row r="267" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="18">
         <f t="shared" si="2"/>
         <v>265</v>
@@ -22444,7 +22388,7 @@
         <v>35.328188649018855</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="12.75" customHeight="1">
+    <row r="268" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="18">
         <f t="shared" si="2"/>
         <v>266</v>
@@ -22460,7 +22404,7 @@
         <v>35.283233055751865</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="12.75" customHeight="1">
+    <row r="269" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="18">
         <f t="shared" si="2"/>
         <v>267</v>
@@ -22476,7 +22420,7 @@
         <v>35.239288359812718</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="12.75" customHeight="1">
+    <row r="270" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="18">
         <f t="shared" si="2"/>
         <v>268</v>
@@ -22492,7 +22436,7 @@
         <v>35.194701466380579</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="12.75" customHeight="1">
+    <row r="271" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="18">
         <f t="shared" si="2"/>
         <v>269</v>
@@ -22508,7 +22452,7 @@
         <v>35.152081756617086</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="12.75" customHeight="1">
+    <row r="272" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="18">
         <f t="shared" si="2"/>
         <v>270</v>
@@ -22524,7 +22468,7 @@
         <v>35.109703672629614</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="12.75" customHeight="1">
+    <row r="273" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="18">
         <f t="shared" si="2"/>
         <v>271</v>
@@ -22540,7 +22484,7 @@
         <v>35.067933551771205</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="12.75" customHeight="1">
+    <row r="274" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="18">
         <f t="shared" si="2"/>
         <v>272</v>
@@ -22556,7 +22500,7 @@
         <v>35.027867619595575</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="12.75" customHeight="1">
+    <row r="275" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="18">
         <f t="shared" si="2"/>
         <v>273</v>
@@ -22572,7 +22516,7 @@
         <v>34.987655647509143</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="12.75" customHeight="1">
+    <row r="276" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="18">
         <f t="shared" si="2"/>
         <v>274</v>
@@ -22588,7 +22532,7 @@
         <v>34.944671499452539</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="12.75" customHeight="1">
+    <row r="277" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="18">
         <f t="shared" si="2"/>
         <v>275</v>
@@ -22604,7 +22548,7 @@
         <v>34.902363601163621</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="12.75" customHeight="1">
+    <row r="278" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="18">
         <f t="shared" si="2"/>
         <v>276</v>
@@ -22620,7 +22564,7 @@
         <v>34.860434747246366</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="12.75" customHeight="1">
+    <row r="279" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="18">
         <f t="shared" si="2"/>
         <v>277</v>
@@ -22636,7 +22580,7 @@
         <v>34.818953036389878</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="12.75" customHeight="1">
+    <row r="280" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="18">
         <f t="shared" si="2"/>
         <v>278</v>
@@ -22652,7 +22596,7 @@
         <v>34.778740972913653</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="12.75" customHeight="1">
+    <row r="281" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="18">
         <f t="shared" si="2"/>
         <v>279</v>
@@ -22668,7 +22612,7 @@
         <v>34.740573439534039</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="12.75" customHeight="1">
+    <row r="282" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="18">
         <f t="shared" si="2"/>
         <v>280</v>
@@ -22684,7 +22628,7 @@
         <v>34.703321389642845</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="12.75" customHeight="1">
+    <row r="283" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="18">
         <f t="shared" si="2"/>
         <v>281</v>
@@ -22700,7 +22644,7 @@
         <v>34.66704622537366</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="12.75" customHeight="1">
+    <row r="284" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="18">
         <f t="shared" si="2"/>
         <v>282</v>
@@ -22716,7 +22660,7 @@
         <v>34.633936132092195</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="12.75" customHeight="1">
+    <row r="285" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="18">
         <f t="shared" si="2"/>
         <v>283</v>
@@ -22732,7 +22676,7 @@
         <v>34.60084802017667</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="12.75" customHeight="1">
+    <row r="286" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="18">
         <f t="shared" si="2"/>
         <v>284</v>
@@ -22748,7 +22692,7 @@
         <v>34.568661932359149</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="12.75" customHeight="1">
+    <row r="287" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="18">
         <f t="shared" si="2"/>
         <v>285</v>
@@ -22764,7 +22708,7 @@
         <v>34.534210486982445</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="12.75" customHeight="1">
+    <row r="288" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="18">
         <f t="shared" si="2"/>
         <v>286</v>
@@ -22780,7 +22724,7 @@
         <v>34.502202755069924</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="12.75" customHeight="1">
+    <row r="289" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="18">
         <f t="shared" si="2"/>
         <v>287</v>
@@ -22796,7 +22740,7 @@
         <v>34.441742116968634</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="12.75" customHeight="1">
+    <row r="290" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="18">
         <f t="shared" si="2"/>
         <v>288</v>
@@ -22812,7 +22756,7 @@
         <v>34.411076347847221</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="12.75" customHeight="1">
+    <row r="291" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="18">
         <f t="shared" si="2"/>
         <v>289</v>
@@ -22828,7 +22772,7 @@
         <v>34.381903071695504</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="12.75" customHeight="1">
+    <row r="292" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="18">
         <f t="shared" si="2"/>
         <v>290</v>
@@ -22844,7 +22788,7 @@
         <v>34.352999957655172</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="12.75" customHeight="1">
+    <row r="293" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="18">
         <f t="shared" si="2"/>
         <v>291</v>
@@ -22860,7 +22804,7 @@
         <v>34.326013703505154</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="12.75" customHeight="1">
+    <row r="294" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="18">
         <f t="shared" si="2"/>
         <v>292</v>
@@ -22876,7 +22820,7 @@
         <v>34.300958862842464</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="12.75" customHeight="1">
+    <row r="295" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="18">
         <f t="shared" si="2"/>
         <v>293</v>
@@ -22892,7 +22836,7 @@
         <v>34.276006784027302</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="12.75" customHeight="1">
+    <row r="296" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="18">
         <f t="shared" si="2"/>
         <v>294</v>
@@ -22908,7 +22852,7 @@
         <v>34.249897918707482</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="12.75" customHeight="1">
+    <row r="297" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="18">
         <f t="shared" si="2"/>
         <v>295</v>
@@ -22924,7 +22868,7 @@
         <v>34.226135552101695</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="12.75" customHeight="1">
+    <row r="298" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="18">
         <f t="shared" si="2"/>
         <v>296</v>
@@ -22940,7 +22884,7 @@
         <v>34.204222931216215</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="12.75" customHeight="1">
+    <row r="299" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="18">
         <f t="shared" si="2"/>
         <v>297</v>
@@ -22956,7 +22900,7 @@
         <v>34.18289558410774</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="12.75" customHeight="1">
+    <row r="300" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="18">
         <f t="shared" si="2"/>
         <v>298</v>
@@ -22972,7 +22916,7 @@
         <v>34.162718082416099</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="12.75" customHeight="1">
+    <row r="301" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="18">
         <f t="shared" si="2"/>
         <v>299</v>
@@ -22988,7 +22932,7 @@
         <v>34.140468189933102</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="12.75" customHeight="1">
+    <row r="302" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="18">
         <f t="shared" si="2"/>
         <v>300</v>
@@ -23004,7 +22948,7 @@
         <v>34.119366627533324</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="12.75" customHeight="1">
+    <row r="303" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="18">
         <f t="shared" si="2"/>
         <v>301</v>
@@ -23020,7 +22964,7 @@
         <v>34.097840490531553</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="12.75" customHeight="1">
+    <row r="304" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="18">
         <f t="shared" si="2"/>
         <v>302</v>
@@ -23036,7 +22980,7 @@
         <v>34.077913866125826</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="12.75" customHeight="1">
+    <row r="305" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="18">
         <f t="shared" si="2"/>
         <v>303</v>
@@ -23052,7 +22996,7 @@
         <v>34.057623722376235</v>
       </c>
     </row>
-    <row r="306" spans="1:4" ht="12.75" customHeight="1">
+    <row r="306" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="18">
         <f t="shared" si="2"/>
         <v>304</v>
@@ -23068,7 +23012,7 @@
         <v>34.036743378157887</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="12.75" customHeight="1">
+    <row r="307" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="18">
         <f t="shared" si="2"/>
         <v>305</v>
@@ -23084,7 +23028,7 @@
         <v>34.0172130717377</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="12.75" customHeight="1">
+    <row r="308" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="18">
         <f t="shared" si="2"/>
         <v>306</v>
@@ -23100,7 +23044,7 @@
         <v>33.997091462385619</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="12.75" customHeight="1">
+    <row r="309" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="18">
         <f t="shared" si="2"/>
         <v>307</v>
@@ -23116,7 +23060,7 @@
         <v>33.975211687882734</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="12.75" customHeight="1">
+    <row r="310" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="18">
         <f t="shared" si="2"/>
         <v>308</v>
@@ -23132,7 +23076,7 @@
         <v>33.951818144935061</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="12.75" customHeight="1">
+    <row r="311" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="18">
         <f t="shared" si="2"/>
         <v>309</v>
@@ -23148,7 +23092,7 @@
         <v>33.929385077993516</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="12.75" customHeight="1">
+    <row r="312" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="18">
         <f t="shared" si="2"/>
         <v>310</v>
@@ -23164,7 +23108,7 @@
         <v>33.90851609090322</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="12.75" customHeight="1">
+    <row r="313" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="18">
         <f t="shared" si="2"/>
         <v>311</v>
@@ -23180,7 +23124,7 @@
         <v>33.886495137138255</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="12.75" customHeight="1">
+    <row r="314" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="18">
         <f t="shared" si="2"/>
         <v>312</v>
@@ -23196,7 +23140,7 @@
         <v>33.865480729391024</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="12.75" customHeight="1">
+    <row r="315" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="18">
         <f t="shared" si="2"/>
         <v>313</v>
@@ -23212,7 +23156,7 @@
         <v>33.843706028146961</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="12.75" customHeight="1">
+    <row r="316" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="18">
         <f t="shared" si="2"/>
         <v>314</v>
@@ -23228,7 +23172,7 @@
         <v>33.822292954299357</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="12.75" customHeight="1">
+    <row r="317" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="18">
         <f t="shared" si="2"/>
         <v>315</v>
@@ -23244,7 +23188,7 @@
         <v>33.800285673142845</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="12.75" customHeight="1">
+    <row r="318" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="18">
         <f t="shared" si="2"/>
         <v>316</v>
@@ -23260,7 +23204,7 @@
         <v>33.778132867974676</v>
       </c>
     </row>
-    <row r="319" spans="1:4" ht="12.75" customHeight="1">
+    <row r="319" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="18">
         <f t="shared" si="2"/>
         <v>317</v>
@@ -23276,7 +23220,7 @@
         <v>33.755394277507875</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="12.75" customHeight="1">
+    <row r="320" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="18">
         <f t="shared" si="2"/>
         <v>318</v>
@@ -23292,7 +23236,7 @@
         <v>33.733238946698101</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="12.75" customHeight="1">
+    <row r="321" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="18">
         <f t="shared" si="2"/>
         <v>319</v>
@@ -23308,7 +23252,7 @@
         <v>33.710940394639486</v>
       </c>
     </row>
-    <row r="322" spans="1:4" ht="12.75" customHeight="1">
+    <row r="322" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="18">
         <f t="shared" si="2"/>
         <v>320</v>
@@ -23324,7 +23268,7 @@
         <v>33.689062453031241</v>
       </c>
     </row>
-    <row r="323" spans="1:4" ht="12.75" customHeight="1">
+    <row r="323" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="18">
         <f t="shared" si="2"/>
         <v>321</v>
@@ -23340,7 +23284,7 @@
         <v>33.666137024579427</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="12.75" customHeight="1">
+    <row r="324" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="18">
         <f t="shared" si="2"/>
         <v>322</v>
@@ -23356,7 +23300,7 @@
         <v>33.645031011583839</v>
       </c>
     </row>
-    <row r="325" spans="1:4" ht="12.75" customHeight="1">
+    <row r="325" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="18">
         <f t="shared" si="2"/>
         <v>323</v>
@@ -23372,7 +23316,7 @@
         <v>33.622414816501539</v>
       </c>
     </row>
-    <row r="326" spans="1:4" ht="12.75" customHeight="1">
+    <row r="326" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="18">
         <f t="shared" si="2"/>
         <v>324</v>
@@ -23388,7 +23332,7 @@
         <v>33.59876538805554</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="12.75" customHeight="1">
+    <row r="327" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="18">
         <f t="shared" si="2"/>
         <v>325</v>
@@ -23404,7 +23348,7 @@
         <v>33.575630725323066</v>
       </c>
     </row>
-    <row r="328" spans="1:4" ht="12.75" customHeight="1">
+    <row r="328" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="18">
         <f t="shared" si="2"/>
         <v>326</v>
@@ -23420,7 +23364,7 @@
         <v>33.55380363438649</v>
       </c>
     </row>
-    <row r="329" spans="1:4" ht="12.75" customHeight="1">
+    <row r="329" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="18">
         <f t="shared" si="2"/>
         <v>327</v>
@@ -23436,7 +23380,7 @@
         <v>33.532079466574906</v>
       </c>
     </row>
-    <row r="330" spans="1:4" ht="12.75" customHeight="1">
+    <row r="330" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="18">
         <f t="shared" si="2"/>
         <v>328</v>
@@ -23452,7 +23396,7 @@
         <v>33.510823125121938</v>
       </c>
     </row>
-    <row r="331" spans="1:4" ht="12.75" customHeight="1">
+    <row r="331" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="18">
         <f t="shared" si="2"/>
         <v>329</v>
@@ -23468,7 +23412,7 @@
         <v>33.4886017805471</v>
       </c>
     </row>
-    <row r="332" spans="1:4" ht="12.75" customHeight="1">
+    <row r="332" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="18">
         <f t="shared" si="2"/>
         <v>330</v>
@@ -23484,7 +23428,7 @@
         <v>33.468363593333315</v>
       </c>
     </row>
-    <row r="333" spans="1:4" ht="12.75" customHeight="1">
+    <row r="333" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="18">
         <f t="shared" si="2"/>
         <v>331</v>
@@ -23500,7 +23444,7 @@
         <v>33.447673675649533</v>
       </c>
     </row>
-    <row r="334" spans="1:4" ht="12.75" customHeight="1">
+    <row r="334" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="18">
         <f t="shared" si="2"/>
         <v>332</v>
@@ -23516,7 +23460,7 @@
         <v>33.427379475060221</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="12.75" customHeight="1">
+    <row r="335" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="18">
         <f t="shared" si="2"/>
         <v>333</v>
@@ -23532,7 +23476,7 @@
         <v>33.407237192282267</v>
       </c>
     </row>
-    <row r="336" spans="1:4" ht="12.75" customHeight="1">
+    <row r="336" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="18">
         <f t="shared" si="2"/>
         <v>334</v>
@@ -23548,7 +23492,7 @@
         <v>33.388532888862258</v>
       </c>
     </row>
-    <row r="337" spans="1:4" ht="12.75" customHeight="1">
+    <row r="337" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="18">
         <f t="shared" si="2"/>
         <v>335</v>
@@ -23564,7 +23508,7 @@
         <v>33.36955219573133</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="12.75" customHeight="1">
+    <row r="338" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="18">
         <f t="shared" si="2"/>
         <v>336</v>
@@ -23580,7 +23524,7 @@
         <v>33.34928566976189</v>
       </c>
     </row>
-    <row r="339" spans="1:4" ht="12.75" customHeight="1">
+    <row r="339" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="18">
         <f t="shared" si="2"/>
         <v>337</v>
@@ -23596,7 +23540,7 @@
         <v>33.330356036646869</v>
       </c>
     </row>
-    <row r="340" spans="1:4" ht="12.75" customHeight="1">
+    <row r="340" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="18">
         <f t="shared" si="2"/>
         <v>338</v>
@@ -23612,7 +23556,7 @@
         <v>33.311212973254428</v>
       </c>
     </row>
-    <row r="341" spans="1:4" ht="12.75" customHeight="1">
+    <row r="341" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="18">
         <f t="shared" si="2"/>
         <v>339</v>
@@ -23628,7 +23572,7 @@
         <v>33.289498482949838</v>
       </c>
     </row>
-    <row r="342" spans="1:4" ht="12.75" customHeight="1">
+    <row r="342" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="18">
         <f t="shared" si="2"/>
         <v>340</v>
@@ -23644,7 +23588,7 @@
         <v>33.267764662764691</v>
       </c>
     </row>
-    <row r="343" spans="1:4" ht="12.75" customHeight="1">
+    <row r="343" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="18">
         <f t="shared" si="2"/>
         <v>341</v>
@@ -23660,7 +23604,7 @@
         <v>33.245806410645152</v>
       </c>
     </row>
-    <row r="344" spans="1:4" ht="12.75" customHeight="1">
+    <row r="344" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="18">
         <f t="shared" si="2"/>
         <v>342</v>
@@ -23676,7 +23620,7 @@
         <v>33.223508733537997</v>
       </c>
     </row>
-    <row r="345" spans="1:4" ht="12.75" customHeight="1">
+    <row r="345" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="18">
         <f t="shared" si="2"/>
         <v>343</v>
@@ -23692,7 +23636,7 @@
         <v>33.200932904985407</v>
       </c>
     </row>
-    <row r="346" spans="1:4" ht="12.75" customHeight="1">
+    <row r="346" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="18">
         <f t="shared" si="2"/>
         <v>344</v>
@@ -23708,7 +23652,7 @@
         <v>33.177616240465106</v>
       </c>
     </row>
-    <row r="347" spans="1:4">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347" s="18">
         <f t="shared" si="2"/>
         <v>345</v>
@@ -23724,7 +23668,7 @@
         <v>33.152985469652158</v>
       </c>
     </row>
-    <row r="348" spans="1:4">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348" s="18">
         <f t="shared" si="2"/>
         <v>346</v>
@@ -23740,7 +23684,7 @@
         <v>33.128364413381483</v>
       </c>
     </row>
-    <row r="349" spans="1:4">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349" s="18">
         <f t="shared" si="2"/>
         <v>347</v>
@@ -23756,7 +23700,7 @@
         <v>33.103412352564824</v>
       </c>
     </row>
-    <row r="350" spans="1:4">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350" s="18">
         <f t="shared" si="2"/>
         <v>348</v>
@@ -23772,7 +23716,7 @@
         <v>33.078804848448264</v>
       </c>
     </row>
-    <row r="351" spans="1:4">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351" s="18">
         <f t="shared" si="2"/>
         <v>349</v>
@@ -23788,7 +23732,7 @@
         <v>33.055026039971331</v>
       </c>
     </row>
-    <row r="352" spans="1:4">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352" s="18">
         <f t="shared" si="2"/>
         <v>350</v>
@@ -23804,7 +23748,7 @@
         <v>33.030411681371412</v>
       </c>
     </row>
-    <row r="353" spans="1:4">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353" s="18">
         <f t="shared" si="2"/>
         <v>351</v>
@@ -23820,7 +23764,7 @@
         <v>33.006878029857532</v>
       </c>
     </row>
-    <row r="354" spans="1:4">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354" s="18">
         <f t="shared" si="2"/>
         <v>352</v>
@@ -23836,7 +23780,7 @@
         <v>32.983932353636348</v>
       </c>
     </row>
-    <row r="355" spans="1:4">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355" s="18">
         <f t="shared" si="2"/>
         <v>353</v>
@@ -23852,9 +23796,9 @@
         <v>32.959955208158625</v>
       </c>
     </row>
-    <row r="356" spans="1:4">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356" s="18">
-        <f t="shared" ref="A356:A443" si="3">A355+1</f>
+        <f t="shared" ref="A356:A427" si="3">A355+1</f>
         <v>354</v>
       </c>
       <c r="B356" s="19" t="s">
@@ -23868,7 +23812,7 @@
         <v>32.934475108700553</v>
       </c>
     </row>
-    <row r="357" spans="1:4">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357" s="18">
         <f t="shared" si="3"/>
         <v>355</v>
@@ -23884,7 +23828,7 @@
         <v>32.90789912247886</v>
       </c>
     </row>
-    <row r="358" spans="1:4">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358" s="18">
         <f t="shared" si="3"/>
         <v>356</v>
@@ -23900,7 +23844,7 @@
         <v>32.881472439550549</v>
       </c>
     </row>
-    <row r="359" spans="1:4">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359" s="18">
         <f t="shared" si="3"/>
         <v>357</v>
@@ -23916,7 +23860,7 @@
         <v>32.85519380526609</v>
       </c>
     </row>
-    <row r="360" spans="1:4">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360" s="18">
         <f t="shared" si="3"/>
         <v>358</v>
@@ -23932,7 +23876,7 @@
         <v>32.8285871186592</v>
       </c>
     </row>
-    <row r="361" spans="1:4">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361" s="18">
         <f t="shared" si="3"/>
         <v>359</v>
@@ -23948,7 +23892,7 @@
         <v>32.801348714428954</v>
       </c>
     </row>
-    <row r="362" spans="1:4">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362" s="18">
         <f t="shared" si="3"/>
         <v>360</v>
@@ -23964,7 +23908,7 @@
         <v>32.773872745777759</v>
       </c>
     </row>
-    <row r="363" spans="1:4">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363" s="18">
         <f t="shared" si="3"/>
         <v>361</v>
@@ -23980,7 +23924,7 @@
         <v>32.746798306038762</v>
       </c>
     </row>
-    <row r="364" spans="1:4">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364" s="18">
         <f t="shared" si="3"/>
         <v>362</v>
@@ -23996,7 +23940,7 @@
         <v>32.721144167071806</v>
       </c>
     </row>
-    <row r="365" spans="1:4">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365" s="18">
         <f t="shared" si="3"/>
         <v>363</v>
@@ -24012,7 +23956,7 @@
         <v>32.694171318126706</v>
       </c>
     </row>
-    <row r="366" spans="1:4">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366" s="18">
         <f t="shared" si="3"/>
         <v>364</v>
@@ -24028,7 +23972,7 @@
         <v>32.66762139881866</v>
       </c>
     </row>
-    <row r="367" spans="1:4">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367" s="18">
         <f t="shared" si="3"/>
         <v>365</v>
@@ -24044,7 +23988,7 @@
         <v>32.640066271698615</v>
       </c>
     </row>
-    <row r="368" spans="1:4">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368" s="18">
         <f t="shared" si="3"/>
         <v>366</v>
@@ -24060,7 +24004,7 @@
         <v>32.611104344508178</v>
       </c>
     </row>
-    <row r="369" spans="1:4">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369" s="18">
         <f t="shared" si="3"/>
         <v>367</v>
@@ -24076,7 +24020,7 @@
         <v>32.582845203978181</v>
       </c>
     </row>
-    <row r="370" spans="1:4">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A370" s="18">
         <f t="shared" si="3"/>
         <v>368</v>
@@ -24092,7 +24036,7 @@
         <v>32.556587472663026</v>
       </c>
     </row>
-    <row r="371" spans="1:4">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A371" s="18">
         <f t="shared" si="3"/>
         <v>369</v>
@@ -24108,7 +24052,7 @@
         <v>32.530282358590767</v>
       </c>
     </row>
-    <row r="372" spans="1:4">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A372" s="18">
         <f t="shared" si="3"/>
         <v>370</v>
@@ -24124,7 +24068,7 @@
         <v>32.506281594432416</v>
       </c>
     </row>
-    <row r="373" spans="1:4">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A373" s="18">
         <f t="shared" si="3"/>
         <v>371</v>
@@ -24140,7 +24084,7 @@
         <v>32.482598892857126</v>
       </c>
     </row>
-    <row r="374" spans="1:4">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374" s="18">
         <f t="shared" si="3"/>
         <v>372</v>
@@ -24156,7 +24100,7 @@
         <v>32.459392982876324</v>
       </c>
     </row>
-    <row r="375" spans="1:4">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A375" s="18">
         <f t="shared" si="3"/>
         <v>373</v>
@@ -24172,7 +24116,7 @@
         <v>32.435614449812313</v>
       </c>
     </row>
-    <row r="376" spans="1:4">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376" s="18">
         <f t="shared" si="3"/>
         <v>374</v>
@@ -24188,7 +24132,7 @@
         <v>32.411455051871634</v>
       </c>
     </row>
-    <row r="377" spans="1:4">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377" s="18">
         <f t="shared" si="3"/>
         <v>375</v>
@@ -24204,7 +24148,7 @@
         <v>32.387264505466646</v>
       </c>
     </row>
-    <row r="378" spans="1:4">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378" s="18">
         <f t="shared" si="3"/>
         <v>376</v>
@@ -24220,7 +24164,7 @@
         <v>32.361846248590403</v>
       </c>
     </row>
-    <row r="379" spans="1:4">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379" s="18">
         <f t="shared" si="3"/>
         <v>377</v>
@@ -24236,7 +24180,7 @@
         <v>32.336324109389899</v>
       </c>
     </row>
-    <row r="380" spans="1:4">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380" s="18">
         <f t="shared" si="3"/>
         <v>378</v>
@@ -24252,7 +24196,7 @@
         <v>32.312101030555532</v>
       </c>
     </row>
-    <row r="381" spans="1:4">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381" s="18">
         <f t="shared" si="3"/>
         <v>379</v>
@@ -24268,7 +24212,7 @@
         <v>32.287425299815283</v>
       </c>
     </row>
-    <row r="382" spans="1:4">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382" s="18">
         <f t="shared" si="3"/>
         <v>380</v>
@@ -24284,7 +24228,7 @@
         <v>32.260721547421028</v>
       </c>
     </row>
-    <row r="383" spans="1:4">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383" s="18">
         <f t="shared" si="3"/>
         <v>381</v>
@@ -24300,7 +24244,7 @@
         <v>32.234420440393677</v>
       </c>
     </row>
-    <row r="384" spans="1:4">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384" s="18">
         <f t="shared" si="3"/>
         <v>382</v>
@@ -24316,7 +24260,7 @@
         <v>32.208335571335049</v>
       </c>
     </row>
-    <row r="385" spans="1:4">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385" s="18">
         <f t="shared" si="3"/>
         <v>383</v>
@@ -24332,7 +24276,7 @@
         <v>32.183248534281958</v>
       </c>
     </row>
-    <row r="386" spans="1:4">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386" s="18">
         <f t="shared" si="3"/>
         <v>384</v>
@@ -24348,7 +24292,7 @@
         <v>32.157979656692682</v>
       </c>
     </row>
-    <row r="387" spans="1:4">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387" s="18">
         <f t="shared" si="3"/>
         <v>385</v>
@@ -24364,7 +24308,7 @@
         <v>32.134712179038935</v>
       </c>
     </row>
-    <row r="388" spans="1:4">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388" s="18">
         <f t="shared" si="3"/>
         <v>386</v>
@@ -24380,7 +24324,7 @@
         <v>32.111539350932617</v>
       </c>
     </row>
-    <row r="389" spans="1:4">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389" s="18">
         <f t="shared" si="3"/>
         <v>387</v>
@@ -24396,7 +24340,7 @@
         <v>32.088072842764831</v>
       </c>
     </row>
-    <row r="390" spans="1:4">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390" s="18">
         <f t="shared" si="3"/>
         <v>388</v>
@@ -24412,7 +24356,7 @@
         <v>32.064031418505131</v>
       </c>
     </row>
-    <row r="391" spans="1:4">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391" s="18">
         <f t="shared" si="3"/>
         <v>389</v>
@@ -24428,7 +24372,7 @@
         <v>32.038982493753188</v>
       </c>
     </row>
-    <row r="392" spans="1:4">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392" s="18">
         <f t="shared" si="3"/>
         <v>390</v>
@@ -24444,7 +24388,7 @@
         <v>32.015472284384586</v>
       </c>
     </row>
-    <row r="393" spans="1:4">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393" s="18">
         <f t="shared" si="3"/>
         <v>391</v>
@@ -24460,7 +24404,7 @@
         <v>31.992133479028105</v>
       </c>
     </row>
-    <row r="394" spans="1:4">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394" s="18">
         <f t="shared" si="3"/>
         <v>392</v>
@@ -24476,7 +24420,7 @@
         <v>31.970342324132627</v>
       </c>
     </row>
-    <row r="395" spans="1:4">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395" s="18">
         <f t="shared" si="3"/>
         <v>393</v>
@@ -24492,7 +24436,7 @@
         <v>31.947847812264605</v>
       </c>
     </row>
-    <row r="396" spans="1:4">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396" s="18">
         <f t="shared" si="3"/>
         <v>394</v>
@@ -24508,7 +24452,7 @@
         <v>31.925162919923835</v>
       </c>
     </row>
-    <row r="397" spans="1:4">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397" s="18">
         <f t="shared" si="3"/>
         <v>395</v>
@@ -24524,7 +24468,7 @@
         <v>31.902643521873394</v>
       </c>
     </row>
-    <row r="398" spans="1:4">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398" s="18">
         <f t="shared" si="3"/>
         <v>396</v>
@@ -24540,7 +24484,7 @@
         <v>31.880162098838358</v>
       </c>
     </row>
-    <row r="399" spans="1:4">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399" s="18">
         <f t="shared" si="3"/>
         <v>397</v>
@@ -24556,7 +24500,7 @@
         <v>31.856912319294686</v>
       </c>
     </row>
-    <row r="400" spans="1:4">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400" s="18">
         <f t="shared" si="3"/>
         <v>398</v>
@@ -24572,7 +24516,7 @@
         <v>31.833502994170832</v>
       </c>
     </row>
-    <row r="401" spans="1:4">
+    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A401" s="18">
         <f t="shared" si="3"/>
         <v>399</v>
@@ -24588,7 +24532,7 @@
         <v>31.810135819323285</v>
       </c>
     </row>
-    <row r="402" spans="1:4">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A402" s="18">
         <f t="shared" si="3"/>
         <v>400</v>
@@ -24604,7 +24548,7 @@
         <v>31.786510481299977</v>
       </c>
     </row>
-    <row r="403" spans="1:4">
+    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A403" s="18">
         <f t="shared" si="3"/>
         <v>401</v>
@@ -24620,7 +24564,7 @@
         <v>31.762603973266813</v>
       </c>
     </row>
-    <row r="404" spans="1:4">
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A404" s="18">
         <f t="shared" si="3"/>
         <v>402</v>
@@ -24636,7 +24580,7 @@
         <v>31.740060184179082</v>
       </c>
     </row>
-    <row r="405" spans="1:4">
+    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A405" s="18">
         <f t="shared" si="3"/>
         <v>403</v>
@@ -24652,7 +24596,7 @@
         <v>31.717901224590552</v>
       </c>
     </row>
-    <row r="406" spans="1:4">
+    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A406" s="18">
         <f t="shared" si="3"/>
         <v>404</v>
@@ -24668,7 +24612,7 @@
         <v>31.696743053440571</v>
       </c>
     </row>
-    <row r="407" spans="1:4">
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A407" s="18">
         <f t="shared" si="3"/>
         <v>405</v>
@@ -24684,7 +24628,7 @@
         <v>31.675343689580224</v>
       </c>
     </row>
-    <row r="408" spans="1:4">
+    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A408" s="18">
         <f t="shared" si="3"/>
         <v>406</v>
@@ -24700,7 +24644,7 @@
         <v>31.654517718201948</v>
       </c>
     </row>
-    <row r="409" spans="1:4">
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A409" s="18">
         <f t="shared" si="3"/>
         <v>407</v>
@@ -24716,7 +24660,7 @@
         <v>31.634383765773933</v>
       </c>
     </row>
-    <row r="410" spans="1:4">
+    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A410" s="18">
         <f t="shared" si="3"/>
         <v>408</v>
@@ -24732,7 +24676,7 @@
         <v>31.614814196789194</v>
       </c>
     </row>
-    <row r="411" spans="1:4">
+    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A411" s="18">
         <f t="shared" si="3"/>
         <v>409</v>
@@ -24748,7 +24692,7 @@
         <v>31.595291421638123</v>
       </c>
     </row>
-    <row r="412" spans="1:4">
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A412" s="18">
         <f t="shared" si="3"/>
         <v>410</v>
@@ -24764,7 +24708,7 @@
         <v>31.576376077073149</v>
       </c>
     </row>
-    <row r="413" spans="1:4">
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A413" s="18">
         <f t="shared" si="3"/>
         <v>411</v>
@@ -24780,7 +24724,7 @@
         <v>31.556968836934285</v>
       </c>
     </row>
-    <row r="414" spans="1:4">
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A414" s="18">
         <f t="shared" si="3"/>
         <v>412</v>
@@ -24796,7 +24740,7 @@
         <v>31.537000465776678</v>
       </c>
     </row>
-    <row r="415" spans="1:4">
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A415" s="18">
         <f t="shared" si="3"/>
         <v>413</v>
@@ -24812,7 +24756,7 @@
         <v>31.51698351661015</v>
       </c>
     </row>
-    <row r="416" spans="1:4">
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A416" s="18">
         <f t="shared" si="3"/>
         <v>414</v>
@@ -24828,7 +24772,7 @@
         <v>31.497618822125581</v>
       </c>
     </row>
-    <row r="417" spans="1:4">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A417" s="18">
         <f t="shared" si="3"/>
         <v>415</v>
@@ -24844,7 +24788,7 @@
         <v>31.477986006602389</v>
       </c>
     </row>
-    <row r="418" spans="1:4">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A418" s="18">
         <f t="shared" si="3"/>
         <v>416</v>
@@ -24860,7 +24804,7 @@
         <v>31.457798540048056</v>
       </c>
     </row>
-    <row r="419" spans="1:4">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A419" s="18">
         <f t="shared" si="3"/>
         <v>417</v>
@@ -24876,7 +24820,7 @@
         <v>31.436820603693025</v>
       </c>
     </row>
-    <row r="420" spans="1:4">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A420" s="18">
         <f t="shared" si="3"/>
         <v>418</v>
@@ -24892,7 +24836,7 @@
         <v>31.415703809449742</v>
       </c>
     </row>
-    <row r="421" spans="1:4">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A421" s="18">
         <f t="shared" si="3"/>
         <v>419</v>
@@ -24908,7 +24852,7 @@
         <v>31.394544609999983</v>
       </c>
     </row>
-    <row r="422" spans="1:4">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A422" s="18">
         <f t="shared" si="3"/>
         <v>420</v>
@@ -24924,7 +24868,7 @@
         <v>31.373248077023792</v>
       </c>
     </row>
-    <row r="423" spans="1:4">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A423" s="18">
         <f t="shared" si="3"/>
         <v>421</v>
@@ -24940,7 +24884,7 @@
         <v>31.352860316555802</v>
       </c>
     </row>
-    <row r="424" spans="1:4">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A424" s="18">
         <f t="shared" si="3"/>
         <v>422</v>
@@ -24956,7 +24900,7 @@
         <v>31.333066808696664</v>
       </c>
     </row>
-    <row r="425" spans="1:4">
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A425" s="18">
         <f t="shared" si="3"/>
         <v>423</v>
@@ -24972,7 +24916,7 @@
         <v>31.312728588203292</v>
       </c>
     </row>
-    <row r="426" spans="1:4">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A426" s="18">
         <f t="shared" si="3"/>
         <v>424</v>
@@ -24988,7 +24932,7 @@
         <v>31.292557059056588</v>
       </c>
     </row>
-    <row r="427" spans="1:4">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A427" s="18">
         <f t="shared" si="3"/>
         <v>425</v>
@@ -25002,262 +24946,6 @@
       <c r="D427" s="18">
         <f>SUM(C$3:C427)/A427</f>
         <v>31.272433394847042</v>
-      </c>
-    </row>
-    <row r="428" spans="1:4">
-      <c r="A428" s="18">
-        <f t="shared" si="3"/>
-        <v>426</v>
-      </c>
-      <c r="B428" s="19" t="s">
-        <v>270</v>
-      </c>
-      <c r="C428" s="20">
-        <v>22.829999919999999</v>
-      </c>
-      <c r="D428" s="18">
-        <f>SUM(C$3:C428)/A428</f>
-        <v>31.252615475892004</v>
-      </c>
-    </row>
-    <row r="429" spans="1:4">
-      <c r="A429" s="18">
-        <f t="shared" si="3"/>
-        <v>427</v>
-      </c>
-      <c r="B429" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="C429" s="20">
-        <v>23.409999849999998</v>
-      </c>
-      <c r="D429" s="18">
-        <f>SUM(C$3:C429)/A429</f>
-        <v>31.234248694566734</v>
-      </c>
-    </row>
-    <row r="430" spans="1:4">
-      <c r="A430" s="18">
-        <f t="shared" si="3"/>
-        <v>428</v>
-      </c>
-      <c r="B430" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="C430" s="20">
-        <v>23.5</v>
-      </c>
-      <c r="D430" s="18">
-        <f>SUM(C$3:C430)/A430</f>
-        <v>31.216178020046716</v>
-      </c>
-    </row>
-    <row r="431" spans="1:4">
-      <c r="A431" s="18">
-        <f t="shared" si="3"/>
-        <v>429</v>
-      </c>
-      <c r="B431" s="19" t="s">
-        <v>273</v>
-      </c>
-      <c r="C431" s="20">
-        <v>23.579999919999999</v>
-      </c>
-      <c r="D431" s="18">
-        <f>SUM(C$3:C431)/A431</f>
-        <v>31.198378071095561</v>
-      </c>
-    </row>
-    <row r="432" spans="1:4">
-      <c r="A432" s="18">
-        <f t="shared" si="3"/>
-        <v>430</v>
-      </c>
-      <c r="B432" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="C432" s="20">
-        <v>23.81999969</v>
-      </c>
-      <c r="D432" s="18">
-        <f>SUM(C$3:C432)/A432</f>
-        <v>31.181219051604643</v>
-      </c>
-    </row>
-    <row r="433" spans="1:4">
-      <c r="A433" s="18">
-        <f t="shared" si="3"/>
-        <v>431</v>
-      </c>
-      <c r="B433" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="C433" s="20">
-        <v>23.649999619999999</v>
-      </c>
-      <c r="D433" s="18">
-        <f>SUM(C$3:C433)/A433</f>
-        <v>31.163745224617159</v>
-      </c>
-    </row>
-    <row r="434" spans="1:4">
-      <c r="A434" s="18">
-        <f t="shared" si="3"/>
-        <v>432</v>
-      </c>
-      <c r="B434" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="C434" s="20">
-        <v>23.780000690000001</v>
-      </c>
-      <c r="D434" s="18">
-        <f>SUM(C$3:C434)/A434</f>
-        <v>31.146653223379619</v>
-      </c>
-    </row>
-    <row r="435" spans="1:4">
-      <c r="A435" s="18">
-        <f t="shared" si="3"/>
-        <v>433</v>
-      </c>
-      <c r="B435" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="C435" s="20">
-        <v>24.100000380000001</v>
-      </c>
-      <c r="D435" s="18">
-        <f>SUM(C$3:C435)/A435</f>
-        <v>31.13037919833717</v>
-      </c>
-    </row>
-    <row r="436" spans="1:4">
-      <c r="A436" s="18">
-        <f t="shared" si="3"/>
-        <v>434</v>
-      </c>
-      <c r="B436" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="C436" s="20">
-        <v>24.450000760000002</v>
-      </c>
-      <c r="D436" s="18">
-        <f>SUM(C$3:C436)/A436</f>
-        <v>31.114986621290313</v>
-      </c>
-    </row>
-    <row r="437" spans="1:4">
-      <c r="A437" s="18">
-        <f t="shared" si="3"/>
-        <v>435</v>
-      </c>
-      <c r="B437" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="C437" s="20">
-        <v>24.520000459999999</v>
-      </c>
-      <c r="D437" s="18">
-        <f>SUM(C$3:C437)/A437</f>
-        <v>31.099825733563208</v>
-      </c>
-    </row>
-    <row r="438" spans="1:4">
-      <c r="A438" s="18">
-        <f t="shared" si="3"/>
-        <v>436</v>
-      </c>
-      <c r="B438" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="C438" s="20">
-        <v>24.530000690000001</v>
-      </c>
-      <c r="D438" s="18">
-        <f>SUM(C$3:C438)/A438</f>
-        <v>31.084757327499986</v>
-      </c>
-    </row>
-    <row r="439" spans="1:4">
-      <c r="A439" s="18">
-        <f t="shared" si="3"/>
-        <v>437</v>
-      </c>
-      <c r="B439" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="C439" s="20">
-        <v>24.739999770000001</v>
-      </c>
-      <c r="D439" s="18">
-        <f>SUM(C$3:C439)/A439</f>
-        <v>31.0702384314874</v>
-      </c>
-    </row>
-    <row r="440" spans="1:4">
-      <c r="A440" s="18">
-        <f t="shared" si="3"/>
-        <v>438</v>
-      </c>
-      <c r="B440" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="C440" s="20">
-        <v>24.829999919999999</v>
-      </c>
-      <c r="D440" s="18">
-        <f>SUM(C$3:C440)/A440</f>
-        <v>31.055991311598159</v>
-      </c>
-    </row>
-    <row r="441" spans="1:4">
-      <c r="A441" s="18">
-        <f t="shared" si="3"/>
-        <v>439</v>
-      </c>
-      <c r="B441" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="C441" s="20">
-        <v>25.170000080000001</v>
-      </c>
-      <c r="D441" s="18">
-        <f>SUM(C$3:C441)/A441</f>
-        <v>31.042583586697024</v>
-      </c>
-    </row>
-    <row r="442" spans="1:4">
-      <c r="A442" s="18">
-        <f t="shared" si="3"/>
-        <v>440</v>
-      </c>
-      <c r="B442" s="19">
-        <v>44956</v>
-      </c>
-      <c r="C442" s="20">
-        <v>24.899999619999999</v>
-      </c>
-      <c r="D442" s="18">
-        <f>SUM(C$3:C442)/A442</f>
-        <v>31.028623168590894</v>
-      </c>
-    </row>
-    <row r="443" spans="1:4">
-      <c r="A443" s="18">
-        <f t="shared" si="3"/>
-        <v>441</v>
-      </c>
-      <c r="B443" s="19">
-        <v>44957</v>
-      </c>
-      <c r="C443" s="20">
-        <v>24.899999619999999</v>
-      </c>
-      <c r="D443" s="18">
-        <f>SUM(C$3:C443)/A443</f>
-        <v>31.014726063038534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>